<commit_message>
old script now works with added features
</commit_message>
<xml_diff>
--- a/1548025318.5751357_statdata.xlsx
+++ b/1548025318.5751357_statdata.xlsx
@@ -29,16 +29,16 @@
     <t>information impact</t>
   </si>
   <si>
-    <t>deg_w</t>
+    <t>$c_i^{deg}$</t>
   </si>
   <si>
-    <t>bet</t>
+    <t>$c_i^{betw}$</t>
   </si>
   <si>
-    <t>ic</t>
+    <t>$c_i^{ic}$</t>
   </si>
   <si>
-    <t>ev</t>
+    <t>$c_i^{ev}$</t>
   </si>
   <si>
     <t>mean</t>
@@ -1111,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="C2">
         <v>0.7833333333333333</v>
@@ -1131,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.9797958971132712</v>
+        <v>0.9637888196533971</v>
       </c>
       <c r="C3">
         <v>0.8239471396205518</v>

</xml_diff>